<commit_message>
Reverse an array question solved!
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bablove/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Love babbar problem set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A296DB3B-D750-F440-AE8C-C019300B98C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527FB431-BFB5-40DE-9CFA-BDD23124D893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16200" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1426,6 +1420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1858,17 +1855,17 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="2" width="123" customWidth="1"/>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26">
+    <row r="1" spans="1:3" ht="24.6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1902,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">

</xml_diff>

<commit_message>
soled maximum and minimum of an array using minimum number of comparisons
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Love babbar problem set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527FB431-BFB5-40DE-9CFA-BDD23124D893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8163C5B9-E178-490B-AFFB-07F5FF05DAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1910,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved find the kth min and max element of an array!
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Love babbar problem set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8163C5B9-E178-490B-AFFB-07F5FF05DAF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08E3E1-033B-415A-995E-8ACE0A1E723B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1887,9 +1887,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="C5" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="5" t="s">
@@ -1921,7 +1919,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">

</xml_diff>